<commit_message>
tabeller update, mit einfacher eingabe der einheiten, formelzeichen und caption
</commit_message>
<xml_diff>
--- a/Tabeller_Vorlage.xlsx
+++ b/Tabeller_Vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balgatim\latex-tabeller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34656968-89B0-4C10-819A-2FF08D439743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F096213-3B72-4F6F-9553-88EB99BC0F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D33979-0E6B-44DA-A425-84AA830345C8}"/>
   </bookViews>
@@ -36,12 +36,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>HEADER 3</t>
+  </si>
+  <si>
+    <t>HEADER 4</t>
+  </si>
+  <si>
+    <t>HEADER 5</t>
+  </si>
+  <si>
+    <t>HEADER 6</t>
+  </si>
+  <si>
+    <t>HEADER 7</t>
+  </si>
+  <si>
+    <t>HEADER 8</t>
+  </si>
+  <si>
+    <t>HEADER 9</t>
+  </si>
+  <si>
+    <t>HEADER 10</t>
+  </si>
+  <si>
+    <t>HEADER 11</t>
+  </si>
+  <si>
+    <t>HEADER 12</t>
+  </si>
+  <si>
+    <t>HEADER 13</t>
+  </si>
+  <si>
+    <t>HEADER 14</t>
+  </si>
+  <si>
+    <t>HEADER 15</t>
+  </si>
+  <si>
+    <t>HEADER 16</t>
+  </si>
+  <si>
+    <t>HEADER 17</t>
+  </si>
+  <si>
+    <t>HEADER 18</t>
+  </si>
+  <si>
+    <t>HEADER 19</t>
+  </si>
+  <si>
+    <t>HEADER 20</t>
+  </si>
+  <si>
+    <t>HEADER 1</t>
+  </si>
+  <si>
+    <t>HEADER 2</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +113,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -430,7 +497,7 @@
   <dimension ref="A1:AK145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,26 +511,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
@@ -483,6 +590,9 @@
       <c r="AK1" s="2"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
@@ -502,6 +612,9 @@
       <c r="AK2" s="2"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
@@ -4219,32 +4332,13 @@
       <c r="AK145" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c3032618-4d7f-458c-877f-4482583a752b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100121BB807B7133F4E97909F1E9C01581D" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="61d18d9999cc13d434223f9e3875bfe4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40" xmlns:ns3="c3032618-4d7f-458c-877f-4482583a752b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a4acd2033efad1f0dccd4f0684ff0f6" ns2:_="" ns3:_="">
     <xsd:import namespace="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40"/>
@@ -4445,10 +4539,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c3032618-4d7f-458c-877f-4482583a752b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABBE2C1-0B0B-4891-85CC-3124E2C37EEA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97D496CE-223B-4967-8C89-F3A8C84F0D3D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40"/>
+    <ds:schemaRef ds:uri="c3032618-4d7f-458c-877f-4482583a752b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4471,20 +4596,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97D496CE-223B-4967-8C89-F3A8C84F0D3D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABBE2C1-0B0B-4891-85CC-3124E2C37EEA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40"/>
-    <ds:schemaRef ds:uri="c3032618-4d7f-458c-877f-4482583a752b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
wieder alles ok gemacht
</commit_message>
<xml_diff>
--- a/Tabeller_Vorlage.xlsx
+++ b/Tabeller_Vorlage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balgatim\latex-tabeller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F096213-3B72-4F6F-9553-88EB99BC0F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0354F950-13A7-4909-9599-877B1FC46D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D33979-0E6B-44DA-A425-84AA830345C8}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D33979-0E6B-44DA-A425-84AA830345C8}"/>
   </bookViews>
   <sheets>
     <sheet name="WISSENSCHAFTLICH" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>HEADER 3</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>HEADER 2</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -497,20 +500,20 @@
   <dimension ref="A1:AK145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -589,9 +592,12 @@
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -611,9 +617,12 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
@@ -633,7 +642,7 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
@@ -652,7 +661,7 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
@@ -671,7 +680,7 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
@@ -690,7 +699,7 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
@@ -709,7 +718,7 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
@@ -728,7 +737,7 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
@@ -747,7 +756,7 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
@@ -766,7 +775,7 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
@@ -785,7 +794,7 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
@@ -804,7 +813,7 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -823,7 +832,7 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -842,7 +851,7 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
@@ -861,7 +870,7 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
@@ -880,7 +889,7 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
@@ -899,7 +908,7 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
-    <row r="18" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
@@ -918,7 +927,7 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
@@ -937,7 +946,7 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
@@ -956,7 +965,7 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
@@ -975,7 +984,7 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
@@ -994,7 +1003,7 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
     </row>
-    <row r="23" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
@@ -1013,7 +1022,7 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
@@ -1032,7 +1041,7 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
     </row>
-    <row r="25" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
@@ -1051,7 +1060,7 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
     </row>
-    <row r="26" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
@@ -1070,7 +1079,7 @@
       <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
     </row>
-    <row r="27" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
@@ -1089,7 +1098,7 @@
       <c r="AJ27" s="2"/>
       <c r="AK27" s="2"/>
     </row>
-    <row r="28" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
@@ -1108,7 +1117,7 @@
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
     </row>
-    <row r="29" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
@@ -1127,7 +1136,7 @@
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
     </row>
-    <row r="30" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
@@ -1146,7 +1155,7 @@
       <c r="AJ30" s="2"/>
       <c r="AK30" s="2"/>
     </row>
-    <row r="31" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
@@ -1165,7 +1174,7 @@
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
     </row>
-    <row r="32" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
@@ -1184,7 +1193,7 @@
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
     </row>
-    <row r="33" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
@@ -1203,7 +1212,7 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
     </row>
-    <row r="34" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
@@ -1222,7 +1231,7 @@
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
     </row>
-    <row r="35" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
@@ -1241,7 +1250,7 @@
       <c r="AJ35" s="2"/>
       <c r="AK35" s="2"/>
     </row>
-    <row r="36" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
@@ -1260,7 +1269,7 @@
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
     </row>
-    <row r="37" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
@@ -1279,7 +1288,7 @@
       <c r="AJ37" s="2"/>
       <c r="AK37" s="2"/>
     </row>
-    <row r="38" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
       <c r="W38" s="2"/>
@@ -1298,7 +1307,7 @@
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
     </row>
-    <row r="39" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
@@ -1317,7 +1326,7 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
     </row>
-    <row r="40" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
@@ -1336,7 +1345,7 @@
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
     </row>
-    <row r="41" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="41" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
       <c r="W41" s="2"/>
@@ -1355,7 +1364,7 @@
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
     </row>
-    <row r="42" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="42" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
@@ -1374,7 +1383,7 @@
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
     </row>
-    <row r="43" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="43" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
       <c r="W43" s="2"/>
@@ -1393,7 +1402,7 @@
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
     </row>
-    <row r="44" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="44" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
       <c r="W44" s="2"/>
@@ -1412,7 +1421,7 @@
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
     </row>
-    <row r="45" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="45" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
@@ -1431,7 +1440,7 @@
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
     </row>
-    <row r="46" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="46" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
@@ -1450,7 +1459,7 @@
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
     </row>
-    <row r="47" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="47" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
       <c r="W47" s="2"/>
@@ -1469,7 +1478,7 @@
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
     </row>
-    <row r="48" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="48" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
       <c r="W48" s="2"/>
@@ -1488,7 +1497,7 @@
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
     </row>
-    <row r="49" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="49" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
       <c r="W49" s="2"/>
@@ -1507,7 +1516,7 @@
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2"/>
     </row>
-    <row r="50" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="50" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
       <c r="W50" s="2"/>
@@ -1526,7 +1535,7 @@
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
     </row>
-    <row r="51" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="51" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
       <c r="W51" s="2"/>
@@ -1545,7 +1554,7 @@
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
     </row>
-    <row r="52" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="52" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
       <c r="W52" s="2"/>
@@ -1564,7 +1573,7 @@
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
     </row>
-    <row r="53" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="53" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
       <c r="W53" s="2"/>
@@ -1583,7 +1592,7 @@
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
     </row>
-    <row r="54" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="54" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
       <c r="W54" s="2"/>
@@ -1602,7 +1611,7 @@
       <c r="AJ54" s="2"/>
       <c r="AK54" s="2"/>
     </row>
-    <row r="55" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="55" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
       <c r="W55" s="2"/>
@@ -1621,7 +1630,7 @@
       <c r="AJ55" s="2"/>
       <c r="AK55" s="2"/>
     </row>
-    <row r="56" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="56" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
       <c r="W56" s="2"/>
@@ -1640,7 +1649,7 @@
       <c r="AJ56" s="2"/>
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="57" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
       <c r="W57" s="2"/>
@@ -1659,7 +1668,7 @@
       <c r="AJ57" s="2"/>
       <c r="AK57" s="2"/>
     </row>
-    <row r="58" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="58" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
       <c r="W58" s="2"/>
@@ -1678,7 +1687,7 @@
       <c r="AJ58" s="2"/>
       <c r="AK58" s="2"/>
     </row>
-    <row r="59" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="59" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
       <c r="W59" s="2"/>
@@ -1697,7 +1706,7 @@
       <c r="AJ59" s="2"/>
       <c r="AK59" s="2"/>
     </row>
-    <row r="60" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="60" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
       <c r="W60" s="2"/>
@@ -1716,7 +1725,7 @@
       <c r="AJ60" s="2"/>
       <c r="AK60" s="2"/>
     </row>
-    <row r="61" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="61" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
       <c r="W61" s="2"/>
@@ -1735,7 +1744,7 @@
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
     </row>
-    <row r="62" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="62" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
       <c r="W62" s="2"/>
@@ -1754,7 +1763,7 @@
       <c r="AJ62" s="2"/>
       <c r="AK62" s="2"/>
     </row>
-    <row r="63" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
       <c r="W63" s="2"/>
@@ -1773,7 +1782,7 @@
       <c r="AJ63" s="2"/>
       <c r="AK63" s="2"/>
     </row>
-    <row r="64" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
       <c r="W64" s="2"/>
@@ -1792,7 +1801,7 @@
       <c r="AJ64" s="2"/>
       <c r="AK64" s="2"/>
     </row>
-    <row r="65" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
       <c r="W65" s="2"/>
@@ -1811,7 +1820,7 @@
       <c r="AJ65" s="2"/>
       <c r="AK65" s="2"/>
     </row>
-    <row r="66" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
@@ -1830,7 +1839,7 @@
       <c r="AJ66" s="2"/>
       <c r="AK66" s="2"/>
     </row>
-    <row r="67" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
       <c r="W67" s="2"/>
@@ -1849,7 +1858,7 @@
       <c r="AJ67" s="2"/>
       <c r="AK67" s="2"/>
     </row>
-    <row r="68" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
       <c r="W68" s="2"/>
@@ -1868,7 +1877,7 @@
       <c r="AJ68" s="2"/>
       <c r="AK68" s="2"/>
     </row>
-    <row r="69" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
       <c r="W69" s="2"/>
@@ -1887,7 +1896,7 @@
       <c r="AJ69" s="2"/>
       <c r="AK69" s="2"/>
     </row>
-    <row r="70" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U70" s="2"/>
       <c r="V70" s="2"/>
       <c r="W70" s="2"/>
@@ -1906,7 +1915,7 @@
       <c r="AJ70" s="2"/>
       <c r="AK70" s="2"/>
     </row>
-    <row r="71" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U71" s="2"/>
       <c r="V71" s="2"/>
       <c r="W71" s="2"/>
@@ -1925,7 +1934,7 @@
       <c r="AJ71" s="2"/>
       <c r="AK71" s="2"/>
     </row>
-    <row r="72" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
       <c r="W72" s="2"/>
@@ -1944,7 +1953,7 @@
       <c r="AJ72" s="2"/>
       <c r="AK72" s="2"/>
     </row>
-    <row r="73" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U73" s="2"/>
       <c r="V73" s="2"/>
       <c r="W73" s="2"/>
@@ -1963,7 +1972,7 @@
       <c r="AJ73" s="2"/>
       <c r="AK73" s="2"/>
     </row>
-    <row r="74" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U74" s="2"/>
       <c r="V74" s="2"/>
       <c r="W74" s="2"/>
@@ -1982,7 +1991,7 @@
       <c r="AJ74" s="2"/>
       <c r="AK74" s="2"/>
     </row>
-    <row r="75" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="75" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U75" s="2"/>
       <c r="V75" s="2"/>
       <c r="W75" s="2"/>
@@ -2001,7 +2010,7 @@
       <c r="AJ75" s="2"/>
       <c r="AK75" s="2"/>
     </row>
-    <row r="76" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="76" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U76" s="2"/>
       <c r="V76" s="2"/>
       <c r="W76" s="2"/>
@@ -2020,7 +2029,7 @@
       <c r="AJ76" s="2"/>
       <c r="AK76" s="2"/>
     </row>
-    <row r="77" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="77" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U77" s="2"/>
       <c r="V77" s="2"/>
       <c r="W77" s="2"/>
@@ -2039,7 +2048,7 @@
       <c r="AJ77" s="2"/>
       <c r="AK77" s="2"/>
     </row>
-    <row r="78" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="78" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U78" s="2"/>
       <c r="V78" s="2"/>
       <c r="W78" s="2"/>
@@ -2058,7 +2067,7 @@
       <c r="AJ78" s="2"/>
       <c r="AK78" s="2"/>
     </row>
-    <row r="79" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="79" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U79" s="2"/>
       <c r="V79" s="2"/>
       <c r="W79" s="2"/>
@@ -2077,7 +2086,7 @@
       <c r="AJ79" s="2"/>
       <c r="AK79" s="2"/>
     </row>
-    <row r="80" spans="21:37" x14ac:dyDescent="0.3">
+    <row r="80" spans="21:37" x14ac:dyDescent="0.25">
       <c r="U80" s="2"/>
       <c r="V80" s="2"/>
       <c r="W80" s="2"/>
@@ -2096,7 +2105,7 @@
       <c r="AJ80" s="2"/>
       <c r="AK80" s="2"/>
     </row>
-    <row r="81" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U81" s="2"/>
       <c r="V81" s="2"/>
       <c r="W81" s="2"/>
@@ -2115,7 +2124,7 @@
       <c r="AJ81" s="2"/>
       <c r="AK81" s="2"/>
     </row>
-    <row r="82" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U82" s="2"/>
       <c r="V82" s="2"/>
       <c r="W82" s="2"/>
@@ -2134,7 +2143,7 @@
       <c r="AJ82" s="2"/>
       <c r="AK82" s="2"/>
     </row>
-    <row r="83" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U83" s="2"/>
       <c r="V83" s="2"/>
       <c r="W83" s="2"/>
@@ -2153,7 +2162,7 @@
       <c r="AJ83" s="2"/>
       <c r="AK83" s="2"/>
     </row>
-    <row r="84" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U84" s="2"/>
       <c r="V84" s="2"/>
       <c r="W84" s="2"/>
@@ -2172,7 +2181,7 @@
       <c r="AJ84" s="2"/>
       <c r="AK84" s="2"/>
     </row>
-    <row r="85" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U85" s="2"/>
       <c r="V85" s="2"/>
       <c r="W85" s="2"/>
@@ -2191,7 +2200,7 @@
       <c r="AJ85" s="2"/>
       <c r="AK85" s="2"/>
     </row>
-    <row r="86" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U86" s="2"/>
       <c r="V86" s="2"/>
       <c r="W86" s="2"/>
@@ -2210,7 +2219,7 @@
       <c r="AJ86" s="2"/>
       <c r="AK86" s="2"/>
     </row>
-    <row r="87" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U87" s="2"/>
       <c r="V87" s="2"/>
       <c r="W87" s="2"/>
@@ -2229,7 +2238,7 @@
       <c r="AJ87" s="2"/>
       <c r="AK87" s="2"/>
     </row>
-    <row r="88" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U88" s="2"/>
       <c r="V88" s="2"/>
       <c r="W88" s="2"/>
@@ -2248,7 +2257,7 @@
       <c r="AJ88" s="2"/>
       <c r="AK88" s="2"/>
     </row>
-    <row r="89" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U89" s="2"/>
       <c r="V89" s="2"/>
       <c r="W89" s="2"/>
@@ -2267,7 +2276,7 @@
       <c r="AJ89" s="2"/>
       <c r="AK89" s="2"/>
     </row>
-    <row r="90" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U90" s="2"/>
       <c r="V90" s="2"/>
       <c r="W90" s="2"/>
@@ -2286,7 +2295,7 @@
       <c r="AJ90" s="2"/>
       <c r="AK90" s="2"/>
     </row>
-    <row r="91" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U91" s="2"/>
       <c r="V91" s="2"/>
       <c r="W91" s="2"/>
@@ -2305,7 +2314,7 @@
       <c r="AJ91" s="2"/>
       <c r="AK91" s="2"/>
     </row>
-    <row r="92" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U92" s="2"/>
       <c r="V92" s="2"/>
       <c r="W92" s="2"/>
@@ -2324,7 +2333,7 @@
       <c r="AJ92" s="2"/>
       <c r="AK92" s="2"/>
     </row>
-    <row r="93" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U93" s="2"/>
       <c r="V93" s="2"/>
       <c r="W93" s="2"/>
@@ -2343,7 +2352,7 @@
       <c r="AJ93" s="2"/>
       <c r="AK93" s="2"/>
     </row>
-    <row r="94" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U94" s="2"/>
       <c r="V94" s="2"/>
       <c r="W94" s="2"/>
@@ -2362,7 +2371,7 @@
       <c r="AJ94" s="2"/>
       <c r="AK94" s="2"/>
     </row>
-    <row r="95" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:37" x14ac:dyDescent="0.25">
       <c r="U95" s="2"/>
       <c r="V95" s="2"/>
       <c r="W95" s="2"/>
@@ -2381,7 +2390,7 @@
       <c r="AJ95" s="2"/>
       <c r="AK95" s="2"/>
     </row>
-    <row r="96" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2420,7 +2429,7 @@
       <c r="AJ96" s="2"/>
       <c r="AK96" s="2"/>
     </row>
-    <row r="97" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2459,7 +2468,7 @@
       <c r="AJ97" s="2"/>
       <c r="AK97" s="2"/>
     </row>
-    <row r="98" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2498,7 +2507,7 @@
       <c r="AJ98" s="2"/>
       <c r="AK98" s="2"/>
     </row>
-    <row r="99" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2537,7 +2546,7 @@
       <c r="AJ99" s="2"/>
       <c r="AK99" s="2"/>
     </row>
-    <row r="100" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2576,7 +2585,7 @@
       <c r="AJ100" s="2"/>
       <c r="AK100" s="2"/>
     </row>
-    <row r="101" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2615,7 +2624,7 @@
       <c r="AJ101" s="2"/>
       <c r="AK101" s="2"/>
     </row>
-    <row r="102" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2654,7 +2663,7 @@
       <c r="AJ102" s="2"/>
       <c r="AK102" s="2"/>
     </row>
-    <row r="103" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2693,7 +2702,7 @@
       <c r="AJ103" s="2"/>
       <c r="AK103" s="2"/>
     </row>
-    <row r="104" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2732,7 +2741,7 @@
       <c r="AJ104" s="2"/>
       <c r="AK104" s="2"/>
     </row>
-    <row r="105" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2771,7 +2780,7 @@
       <c r="AJ105" s="2"/>
       <c r="AK105" s="2"/>
     </row>
-    <row r="106" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2810,7 +2819,7 @@
       <c r="AJ106" s="2"/>
       <c r="AK106" s="2"/>
     </row>
-    <row r="107" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2849,7 +2858,7 @@
       <c r="AJ107" s="2"/>
       <c r="AK107" s="2"/>
     </row>
-    <row r="108" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2888,7 +2897,7 @@
       <c r="AJ108" s="2"/>
       <c r="AK108" s="2"/>
     </row>
-    <row r="109" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2927,7 +2936,7 @@
       <c r="AJ109" s="2"/>
       <c r="AK109" s="2"/>
     </row>
-    <row r="110" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2966,7 +2975,7 @@
       <c r="AJ110" s="2"/>
       <c r="AK110" s="2"/>
     </row>
-    <row r="111" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3005,7 +3014,7 @@
       <c r="AJ111" s="2"/>
       <c r="AK111" s="2"/>
     </row>
-    <row r="112" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3044,7 +3053,7 @@
       <c r="AJ112" s="2"/>
       <c r="AK112" s="2"/>
     </row>
-    <row r="113" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3083,7 +3092,7 @@
       <c r="AJ113" s="2"/>
       <c r="AK113" s="2"/>
     </row>
-    <row r="114" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3122,7 +3131,7 @@
       <c r="AJ114" s="2"/>
       <c r="AK114" s="2"/>
     </row>
-    <row r="115" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3161,7 +3170,7 @@
       <c r="AJ115" s="2"/>
       <c r="AK115" s="2"/>
     </row>
-    <row r="116" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3200,7 +3209,7 @@
       <c r="AJ116" s="2"/>
       <c r="AK116" s="2"/>
     </row>
-    <row r="117" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3239,7 +3248,7 @@
       <c r="AJ117" s="2"/>
       <c r="AK117" s="2"/>
     </row>
-    <row r="118" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3278,7 +3287,7 @@
       <c r="AJ118" s="2"/>
       <c r="AK118" s="2"/>
     </row>
-    <row r="119" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3317,7 +3326,7 @@
       <c r="AJ119" s="2"/>
       <c r="AK119" s="2"/>
     </row>
-    <row r="120" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3356,7 +3365,7 @@
       <c r="AJ120" s="2"/>
       <c r="AK120" s="2"/>
     </row>
-    <row r="121" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3395,7 +3404,7 @@
       <c r="AJ121" s="2"/>
       <c r="AK121" s="2"/>
     </row>
-    <row r="122" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3434,7 +3443,7 @@
       <c r="AJ122" s="2"/>
       <c r="AK122" s="2"/>
     </row>
-    <row r="123" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3473,7 +3482,7 @@
       <c r="AJ123" s="2"/>
       <c r="AK123" s="2"/>
     </row>
-    <row r="124" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3512,7 +3521,7 @@
       <c r="AJ124" s="2"/>
       <c r="AK124" s="2"/>
     </row>
-    <row r="125" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3551,7 +3560,7 @@
       <c r="AJ125" s="2"/>
       <c r="AK125" s="2"/>
     </row>
-    <row r="126" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3590,7 +3599,7 @@
       <c r="AJ126" s="2"/>
       <c r="AK126" s="2"/>
     </row>
-    <row r="127" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3629,7 +3638,7 @@
       <c r="AJ127" s="2"/>
       <c r="AK127" s="2"/>
     </row>
-    <row r="128" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3668,7 +3677,7 @@
       <c r="AJ128" s="2"/>
       <c r="AK128" s="2"/>
     </row>
-    <row r="129" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3707,7 +3716,7 @@
       <c r="AJ129" s="2"/>
       <c r="AK129" s="2"/>
     </row>
-    <row r="130" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3746,7 +3755,7 @@
       <c r="AJ130" s="2"/>
       <c r="AK130" s="2"/>
     </row>
-    <row r="131" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3785,7 +3794,7 @@
       <c r="AJ131" s="2"/>
       <c r="AK131" s="2"/>
     </row>
-    <row r="132" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3824,7 +3833,7 @@
       <c r="AJ132" s="2"/>
       <c r="AK132" s="2"/>
     </row>
-    <row r="133" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3863,7 +3872,7 @@
       <c r="AJ133" s="2"/>
       <c r="AK133" s="2"/>
     </row>
-    <row r="134" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3902,7 +3911,7 @@
       <c r="AJ134" s="2"/>
       <c r="AK134" s="2"/>
     </row>
-    <row r="135" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3941,7 +3950,7 @@
       <c r="AJ135" s="2"/>
       <c r="AK135" s="2"/>
     </row>
-    <row r="136" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3980,7 +3989,7 @@
       <c r="AJ136" s="2"/>
       <c r="AK136" s="2"/>
     </row>
-    <row r="137" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -4019,7 +4028,7 @@
       <c r="AJ137" s="2"/>
       <c r="AK137" s="2"/>
     </row>
-    <row r="138" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -4058,7 +4067,7 @@
       <c r="AJ138" s="2"/>
       <c r="AK138" s="2"/>
     </row>
-    <row r="139" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -4097,7 +4106,7 @@
       <c r="AJ139" s="2"/>
       <c r="AK139" s="2"/>
     </row>
-    <row r="140" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -4136,7 +4145,7 @@
       <c r="AJ140" s="2"/>
       <c r="AK140" s="2"/>
     </row>
-    <row r="141" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -4175,7 +4184,7 @@
       <c r="AJ141" s="2"/>
       <c r="AK141" s="2"/>
     </row>
-    <row r="142" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -4214,7 +4223,7 @@
       <c r="AJ142" s="2"/>
       <c r="AK142" s="2"/>
     </row>
-    <row r="143" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -4253,7 +4262,7 @@
       <c r="AJ143" s="2"/>
       <c r="AK143" s="2"/>
     </row>
-    <row r="144" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -4292,7 +4301,7 @@
       <c r="AJ144" s="2"/>
       <c r="AK144" s="2"/>
     </row>
-    <row r="145" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -4339,6 +4348,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c3032618-4d7f-458c-877f-4482583a752b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100121BB807B7133F4E97909F1E9C01581D" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="61d18d9999cc13d434223f9e3875bfe4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40" xmlns:ns3="c3032618-4d7f-458c-877f-4482583a752b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a4acd2033efad1f0dccd4f0684ff0f6" ns2:_="" ns3:_="">
     <xsd:import namespace="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40"/>
@@ -4539,41 +4568,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c3032618-4d7f-458c-877f-4482583a752b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97D496CE-223B-4967-8C89-F3A8C84F0D3D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABBE2C1-0B0B-4891-85CC-3124E2C37EEA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40"/>
-    <ds:schemaRef ds:uri="c3032618-4d7f-458c-877f-4482583a752b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4596,9 +4594,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABBE2C1-0B0B-4891-85CC-3124E2C37EEA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97D496CE-223B-4967-8C89-F3A8C84F0D3D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40"/>
+    <ds:schemaRef ds:uri="c3032618-4d7f-458c-877f-4482583a752b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
funktioniert gut: auf A4 breite erweitern caption wird richtig übernommen und header wird dynamisch im programm angezeigt
</commit_message>
<xml_diff>
--- a/Tabeller_Vorlage.xlsx
+++ b/Tabeller_Vorlage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balgatim\latex-tabeller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0354F950-13A7-4909-9599-877B1FC46D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982B401D-6A79-4C24-98B3-118A8D8EDA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D33979-0E6B-44DA-A425-84AA830345C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41D33979-0E6B-44DA-A425-84AA830345C8}"/>
   </bookViews>
   <sheets>
     <sheet name="WISSENSCHAFTLICH" sheetId="3" r:id="rId1"/>
@@ -98,13 +98,16 @@
     <t>HEADER 2</t>
   </si>
   <si>
-    <t>e</t>
+    <t>Summe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,10 +162,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -500,20 +504,20 @@
   <dimension ref="A1:AK145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -592,12 +596,16 @@
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
+      <c r="B2" s="3">
+        <f>452.33</f>
+        <v>452.33</v>
+      </c>
+      <c r="C2" s="3">
+        <v>493.29</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -617,12 +625,15 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>489.29</v>
+      </c>
+      <c r="C3" s="3">
+        <v>493.29</v>
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
@@ -642,7 +653,17 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B16" si="0">452.33</f>
+        <v>452.33</v>
+      </c>
+      <c r="C4" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
@@ -661,7 +682,16 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>490.29</v>
+      </c>
+      <c r="C5" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
@@ -680,7 +710,17 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ref="B6:B16" si="1">452.33</f>
+        <v>452.33</v>
+      </c>
+      <c r="C6" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
@@ -699,7 +739,16 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>491.29</v>
+      </c>
+      <c r="C7" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
@@ -718,7 +767,17 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" ref="B8:B16" si="2">452.33</f>
+        <v>452.33</v>
+      </c>
+      <c r="C8" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
@@ -737,7 +796,16 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>492.29</v>
+      </c>
+      <c r="C9" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
@@ -756,7 +824,17 @@
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ref="B10:B16" si="3">452.33</f>
+        <v>452.33</v>
+      </c>
+      <c r="C10" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
@@ -775,7 +853,16 @@
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>493.29</v>
+      </c>
+      <c r="C11" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
@@ -794,7 +881,17 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ref="B12:B16" si="4">452.33</f>
+        <v>452.33</v>
+      </c>
+      <c r="C12" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
@@ -813,7 +910,16 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>494.29</v>
+      </c>
+      <c r="C13" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
@@ -832,7 +938,17 @@
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" ref="B14:B16" si="5">452.33</f>
+        <v>452.33</v>
+      </c>
+      <c r="C14" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
@@ -851,7 +967,16 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>495.29</v>
+      </c>
+      <c r="C15" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
@@ -870,7 +995,17 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" ref="B16" si="6">452.33</f>
+        <v>452.33</v>
+      </c>
+      <c r="C16" s="3">
+        <v>493.29</v>
+      </c>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
@@ -889,7 +1024,18 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
     </row>
-    <row r="17" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3">
+        <f>SUM(B2:B16)</f>
+        <v>7064.67</v>
+      </c>
+      <c r="C17" s="3">
+        <f>SUM(C2:C16)</f>
+        <v>7399.35</v>
+      </c>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
@@ -908,7 +1054,7 @@
       <c r="AJ17" s="2"/>
       <c r="AK17" s="2"/>
     </row>
-    <row r="18" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
@@ -927,7 +1073,7 @@
       <c r="AJ18" s="2"/>
       <c r="AK18" s="2"/>
     </row>
-    <row r="19" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
@@ -946,7 +1092,7 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
     </row>
-    <row r="20" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
@@ -965,7 +1111,7 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
     </row>
-    <row r="21" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
@@ -984,7 +1130,7 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
     </row>
-    <row r="22" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
@@ -1003,7 +1149,7 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
     </row>
-    <row r="23" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
@@ -1022,7 +1168,7 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
     </row>
-    <row r="24" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
@@ -1041,7 +1187,7 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
     </row>
-    <row r="25" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
@@ -1060,7 +1206,7 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
     </row>
-    <row r="26" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
@@ -1079,7 +1225,7 @@
       <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
     </row>
-    <row r="27" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
@@ -1098,7 +1244,7 @@
       <c r="AJ27" s="2"/>
       <c r="AK27" s="2"/>
     </row>
-    <row r="28" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
@@ -1117,7 +1263,7 @@
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
     </row>
-    <row r="29" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
       <c r="W29" s="2"/>
@@ -1136,7 +1282,7 @@
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
     </row>
-    <row r="30" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
       <c r="W30" s="2"/>
@@ -1155,7 +1301,7 @@
       <c r="AJ30" s="2"/>
       <c r="AK30" s="2"/>
     </row>
-    <row r="31" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
       <c r="W31" s="2"/>
@@ -1174,7 +1320,7 @@
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
     </row>
-    <row r="32" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
@@ -1193,7 +1339,7 @@
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
     </row>
-    <row r="33" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
@@ -1212,7 +1358,7 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
     </row>
-    <row r="34" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
@@ -1231,7 +1377,7 @@
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
     </row>
-    <row r="35" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
@@ -1250,7 +1396,7 @@
       <c r="AJ35" s="2"/>
       <c r="AK35" s="2"/>
     </row>
-    <row r="36" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
@@ -1269,7 +1415,7 @@
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
     </row>
-    <row r="37" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
@@ -1288,7 +1434,7 @@
       <c r="AJ37" s="2"/>
       <c r="AK37" s="2"/>
     </row>
-    <row r="38" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
       <c r="W38" s="2"/>
@@ -1307,7 +1453,7 @@
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
     </row>
-    <row r="39" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
@@ -1326,7 +1472,7 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
     </row>
-    <row r="40" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
@@ -1345,7 +1491,7 @@
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
     </row>
-    <row r="41" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
       <c r="W41" s="2"/>
@@ -1364,7 +1510,7 @@
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
     </row>
-    <row r="42" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
@@ -1383,7 +1529,7 @@
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
     </row>
-    <row r="43" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
       <c r="W43" s="2"/>
@@ -1402,7 +1548,7 @@
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
     </row>
-    <row r="44" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
       <c r="W44" s="2"/>
@@ -1421,7 +1567,7 @@
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
     </row>
-    <row r="45" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
@@ -1440,7 +1586,7 @@
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
     </row>
-    <row r="46" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
@@ -1459,7 +1605,7 @@
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
     </row>
-    <row r="47" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
       <c r="W47" s="2"/>
@@ -1478,7 +1624,7 @@
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
     </row>
-    <row r="48" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
       <c r="W48" s="2"/>
@@ -1497,7 +1643,7 @@
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
     </row>
-    <row r="49" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
       <c r="W49" s="2"/>
@@ -1516,7 +1662,7 @@
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2"/>
     </row>
-    <row r="50" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
       <c r="W50" s="2"/>
@@ -1535,7 +1681,7 @@
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
     </row>
-    <row r="51" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
       <c r="W51" s="2"/>
@@ -1554,7 +1700,7 @@
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
     </row>
-    <row r="52" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
       <c r="W52" s="2"/>
@@ -1573,7 +1719,7 @@
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
     </row>
-    <row r="53" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
       <c r="W53" s="2"/>
@@ -1592,7 +1738,7 @@
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
     </row>
-    <row r="54" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
       <c r="W54" s="2"/>
@@ -1611,7 +1757,7 @@
       <c r="AJ54" s="2"/>
       <c r="AK54" s="2"/>
     </row>
-    <row r="55" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
       <c r="W55" s="2"/>
@@ -1630,7 +1776,7 @@
       <c r="AJ55" s="2"/>
       <c r="AK55" s="2"/>
     </row>
-    <row r="56" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
       <c r="W56" s="2"/>
@@ -1649,7 +1795,7 @@
       <c r="AJ56" s="2"/>
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
       <c r="W57" s="2"/>
@@ -1668,7 +1814,7 @@
       <c r="AJ57" s="2"/>
       <c r="AK57" s="2"/>
     </row>
-    <row r="58" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
       <c r="W58" s="2"/>
@@ -1687,7 +1833,7 @@
       <c r="AJ58" s="2"/>
       <c r="AK58" s="2"/>
     </row>
-    <row r="59" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
       <c r="W59" s="2"/>
@@ -1706,7 +1852,7 @@
       <c r="AJ59" s="2"/>
       <c r="AK59" s="2"/>
     </row>
-    <row r="60" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="60" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
       <c r="W60" s="2"/>
@@ -1725,7 +1871,7 @@
       <c r="AJ60" s="2"/>
       <c r="AK60" s="2"/>
     </row>
-    <row r="61" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
       <c r="W61" s="2"/>
@@ -1744,7 +1890,7 @@
       <c r="AJ61" s="2"/>
       <c r="AK61" s="2"/>
     </row>
-    <row r="62" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
       <c r="W62" s="2"/>
@@ -1763,7 +1909,7 @@
       <c r="AJ62" s="2"/>
       <c r="AK62" s="2"/>
     </row>
-    <row r="63" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
       <c r="W63" s="2"/>
@@ -1782,7 +1928,7 @@
       <c r="AJ63" s="2"/>
       <c r="AK63" s="2"/>
     </row>
-    <row r="64" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
       <c r="W64" s="2"/>
@@ -1801,7 +1947,7 @@
       <c r="AJ64" s="2"/>
       <c r="AK64" s="2"/>
     </row>
-    <row r="65" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
       <c r="W65" s="2"/>
@@ -1820,7 +1966,7 @@
       <c r="AJ65" s="2"/>
       <c r="AK65" s="2"/>
     </row>
-    <row r="66" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
@@ -1839,7 +1985,7 @@
       <c r="AJ66" s="2"/>
       <c r="AK66" s="2"/>
     </row>
-    <row r="67" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
       <c r="W67" s="2"/>
@@ -1858,7 +2004,7 @@
       <c r="AJ67" s="2"/>
       <c r="AK67" s="2"/>
     </row>
-    <row r="68" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
       <c r="W68" s="2"/>
@@ -1877,7 +2023,7 @@
       <c r="AJ68" s="2"/>
       <c r="AK68" s="2"/>
     </row>
-    <row r="69" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="69" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
       <c r="W69" s="2"/>
@@ -1896,7 +2042,7 @@
       <c r="AJ69" s="2"/>
       <c r="AK69" s="2"/>
     </row>
-    <row r="70" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U70" s="2"/>
       <c r="V70" s="2"/>
       <c r="W70" s="2"/>
@@ -1915,7 +2061,7 @@
       <c r="AJ70" s="2"/>
       <c r="AK70" s="2"/>
     </row>
-    <row r="71" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="71" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U71" s="2"/>
       <c r="V71" s="2"/>
       <c r="W71" s="2"/>
@@ -1934,7 +2080,7 @@
       <c r="AJ71" s="2"/>
       <c r="AK71" s="2"/>
     </row>
-    <row r="72" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="72" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
       <c r="W72" s="2"/>
@@ -1953,7 +2099,7 @@
       <c r="AJ72" s="2"/>
       <c r="AK72" s="2"/>
     </row>
-    <row r="73" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="73" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U73" s="2"/>
       <c r="V73" s="2"/>
       <c r="W73" s="2"/>
@@ -1972,7 +2118,7 @@
       <c r="AJ73" s="2"/>
       <c r="AK73" s="2"/>
     </row>
-    <row r="74" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="74" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U74" s="2"/>
       <c r="V74" s="2"/>
       <c r="W74" s="2"/>
@@ -1991,7 +2137,7 @@
       <c r="AJ74" s="2"/>
       <c r="AK74" s="2"/>
     </row>
-    <row r="75" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="75" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U75" s="2"/>
       <c r="V75" s="2"/>
       <c r="W75" s="2"/>
@@ -2010,7 +2156,7 @@
       <c r="AJ75" s="2"/>
       <c r="AK75" s="2"/>
     </row>
-    <row r="76" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="76" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U76" s="2"/>
       <c r="V76" s="2"/>
       <c r="W76" s="2"/>
@@ -2029,7 +2175,7 @@
       <c r="AJ76" s="2"/>
       <c r="AK76" s="2"/>
     </row>
-    <row r="77" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="77" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U77" s="2"/>
       <c r="V77" s="2"/>
       <c r="W77" s="2"/>
@@ -2048,7 +2194,7 @@
       <c r="AJ77" s="2"/>
       <c r="AK77" s="2"/>
     </row>
-    <row r="78" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="78" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U78" s="2"/>
       <c r="V78" s="2"/>
       <c r="W78" s="2"/>
@@ -2067,7 +2213,7 @@
       <c r="AJ78" s="2"/>
       <c r="AK78" s="2"/>
     </row>
-    <row r="79" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="79" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U79" s="2"/>
       <c r="V79" s="2"/>
       <c r="W79" s="2"/>
@@ -2086,7 +2232,7 @@
       <c r="AJ79" s="2"/>
       <c r="AK79" s="2"/>
     </row>
-    <row r="80" spans="21:37" x14ac:dyDescent="0.25">
+    <row r="80" spans="21:37" x14ac:dyDescent="0.3">
       <c r="U80" s="2"/>
       <c r="V80" s="2"/>
       <c r="W80" s="2"/>
@@ -2105,7 +2251,7 @@
       <c r="AJ80" s="2"/>
       <c r="AK80" s="2"/>
     </row>
-    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U81" s="2"/>
       <c r="V81" s="2"/>
       <c r="W81" s="2"/>
@@ -2124,7 +2270,7 @@
       <c r="AJ81" s="2"/>
       <c r="AK81" s="2"/>
     </row>
-    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U82" s="2"/>
       <c r="V82" s="2"/>
       <c r="W82" s="2"/>
@@ -2143,7 +2289,7 @@
       <c r="AJ82" s="2"/>
       <c r="AK82" s="2"/>
     </row>
-    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U83" s="2"/>
       <c r="V83" s="2"/>
       <c r="W83" s="2"/>
@@ -2162,7 +2308,7 @@
       <c r="AJ83" s="2"/>
       <c r="AK83" s="2"/>
     </row>
-    <row r="84" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U84" s="2"/>
       <c r="V84" s="2"/>
       <c r="W84" s="2"/>
@@ -2181,7 +2327,7 @@
       <c r="AJ84" s="2"/>
       <c r="AK84" s="2"/>
     </row>
-    <row r="85" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U85" s="2"/>
       <c r="V85" s="2"/>
       <c r="W85" s="2"/>
@@ -2200,7 +2346,7 @@
       <c r="AJ85" s="2"/>
       <c r="AK85" s="2"/>
     </row>
-    <row r="86" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U86" s="2"/>
       <c r="V86" s="2"/>
       <c r="W86" s="2"/>
@@ -2219,7 +2365,7 @@
       <c r="AJ86" s="2"/>
       <c r="AK86" s="2"/>
     </row>
-    <row r="87" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U87" s="2"/>
       <c r="V87" s="2"/>
       <c r="W87" s="2"/>
@@ -2238,7 +2384,7 @@
       <c r="AJ87" s="2"/>
       <c r="AK87" s="2"/>
     </row>
-    <row r="88" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U88" s="2"/>
       <c r="V88" s="2"/>
       <c r="W88" s="2"/>
@@ -2257,7 +2403,7 @@
       <c r="AJ88" s="2"/>
       <c r="AK88" s="2"/>
     </row>
-    <row r="89" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U89" s="2"/>
       <c r="V89" s="2"/>
       <c r="W89" s="2"/>
@@ -2276,7 +2422,7 @@
       <c r="AJ89" s="2"/>
       <c r="AK89" s="2"/>
     </row>
-    <row r="90" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U90" s="2"/>
       <c r="V90" s="2"/>
       <c r="W90" s="2"/>
@@ -2295,7 +2441,7 @@
       <c r="AJ90" s="2"/>
       <c r="AK90" s="2"/>
     </row>
-    <row r="91" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U91" s="2"/>
       <c r="V91" s="2"/>
       <c r="W91" s="2"/>
@@ -2314,7 +2460,7 @@
       <c r="AJ91" s="2"/>
       <c r="AK91" s="2"/>
     </row>
-    <row r="92" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U92" s="2"/>
       <c r="V92" s="2"/>
       <c r="W92" s="2"/>
@@ -2333,7 +2479,7 @@
       <c r="AJ92" s="2"/>
       <c r="AK92" s="2"/>
     </row>
-    <row r="93" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U93" s="2"/>
       <c r="V93" s="2"/>
       <c r="W93" s="2"/>
@@ -2352,7 +2498,7 @@
       <c r="AJ93" s="2"/>
       <c r="AK93" s="2"/>
     </row>
-    <row r="94" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U94" s="2"/>
       <c r="V94" s="2"/>
       <c r="W94" s="2"/>
@@ -2371,7 +2517,7 @@
       <c r="AJ94" s="2"/>
       <c r="AK94" s="2"/>
     </row>
-    <row r="95" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U95" s="2"/>
       <c r="V95" s="2"/>
       <c r="W95" s="2"/>
@@ -2390,7 +2536,7 @@
       <c r="AJ95" s="2"/>
       <c r="AK95" s="2"/>
     </row>
-    <row r="96" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2429,7 +2575,7 @@
       <c r="AJ96" s="2"/>
       <c r="AK96" s="2"/>
     </row>
-    <row r="97" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2468,7 +2614,7 @@
       <c r="AJ97" s="2"/>
       <c r="AK97" s="2"/>
     </row>
-    <row r="98" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2507,7 +2653,7 @@
       <c r="AJ98" s="2"/>
       <c r="AK98" s="2"/>
     </row>
-    <row r="99" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2546,7 +2692,7 @@
       <c r="AJ99" s="2"/>
       <c r="AK99" s="2"/>
     </row>
-    <row r="100" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2585,7 +2731,7 @@
       <c r="AJ100" s="2"/>
       <c r="AK100" s="2"/>
     </row>
-    <row r="101" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2624,7 +2770,7 @@
       <c r="AJ101" s="2"/>
       <c r="AK101" s="2"/>
     </row>
-    <row r="102" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2663,7 +2809,7 @@
       <c r="AJ102" s="2"/>
       <c r="AK102" s="2"/>
     </row>
-    <row r="103" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2702,7 +2848,7 @@
       <c r="AJ103" s="2"/>
       <c r="AK103" s="2"/>
     </row>
-    <row r="104" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2741,7 +2887,7 @@
       <c r="AJ104" s="2"/>
       <c r="AK104" s="2"/>
     </row>
-    <row r="105" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2780,7 +2926,7 @@
       <c r="AJ105" s="2"/>
       <c r="AK105" s="2"/>
     </row>
-    <row r="106" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2819,7 +2965,7 @@
       <c r="AJ106" s="2"/>
       <c r="AK106" s="2"/>
     </row>
-    <row r="107" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2858,7 +3004,7 @@
       <c r="AJ107" s="2"/>
       <c r="AK107" s="2"/>
     </row>
-    <row r="108" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2897,7 +3043,7 @@
       <c r="AJ108" s="2"/>
       <c r="AK108" s="2"/>
     </row>
-    <row r="109" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2936,7 +3082,7 @@
       <c r="AJ109" s="2"/>
       <c r="AK109" s="2"/>
     </row>
-    <row r="110" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2975,7 +3121,7 @@
       <c r="AJ110" s="2"/>
       <c r="AK110" s="2"/>
     </row>
-    <row r="111" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3014,7 +3160,7 @@
       <c r="AJ111" s="2"/>
       <c r="AK111" s="2"/>
     </row>
-    <row r="112" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3053,7 +3199,7 @@
       <c r="AJ112" s="2"/>
       <c r="AK112" s="2"/>
     </row>
-    <row r="113" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3092,7 +3238,7 @@
       <c r="AJ113" s="2"/>
       <c r="AK113" s="2"/>
     </row>
-    <row r="114" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3131,7 +3277,7 @@
       <c r="AJ114" s="2"/>
       <c r="AK114" s="2"/>
     </row>
-    <row r="115" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3170,7 +3316,7 @@
       <c r="AJ115" s="2"/>
       <c r="AK115" s="2"/>
     </row>
-    <row r="116" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3209,7 +3355,7 @@
       <c r="AJ116" s="2"/>
       <c r="AK116" s="2"/>
     </row>
-    <row r="117" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3248,7 +3394,7 @@
       <c r="AJ117" s="2"/>
       <c r="AK117" s="2"/>
     </row>
-    <row r="118" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3287,7 +3433,7 @@
       <c r="AJ118" s="2"/>
       <c r="AK118" s="2"/>
     </row>
-    <row r="119" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3326,7 +3472,7 @@
       <c r="AJ119" s="2"/>
       <c r="AK119" s="2"/>
     </row>
-    <row r="120" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3365,7 +3511,7 @@
       <c r="AJ120" s="2"/>
       <c r="AK120" s="2"/>
     </row>
-    <row r="121" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3404,7 +3550,7 @@
       <c r="AJ121" s="2"/>
       <c r="AK121" s="2"/>
     </row>
-    <row r="122" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3443,7 +3589,7 @@
       <c r="AJ122" s="2"/>
       <c r="AK122" s="2"/>
     </row>
-    <row r="123" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3482,7 +3628,7 @@
       <c r="AJ123" s="2"/>
       <c r="AK123" s="2"/>
     </row>
-    <row r="124" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3521,7 +3667,7 @@
       <c r="AJ124" s="2"/>
       <c r="AK124" s="2"/>
     </row>
-    <row r="125" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3560,7 +3706,7 @@
       <c r="AJ125" s="2"/>
       <c r="AK125" s="2"/>
     </row>
-    <row r="126" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3599,7 +3745,7 @@
       <c r="AJ126" s="2"/>
       <c r="AK126" s="2"/>
     </row>
-    <row r="127" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3638,7 +3784,7 @@
       <c r="AJ127" s="2"/>
       <c r="AK127" s="2"/>
     </row>
-    <row r="128" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3677,7 +3823,7 @@
       <c r="AJ128" s="2"/>
       <c r="AK128" s="2"/>
     </row>
-    <row r="129" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3716,7 +3862,7 @@
       <c r="AJ129" s="2"/>
       <c r="AK129" s="2"/>
     </row>
-    <row r="130" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3755,7 +3901,7 @@
       <c r="AJ130" s="2"/>
       <c r="AK130" s="2"/>
     </row>
-    <row r="131" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3794,7 +3940,7 @@
       <c r="AJ131" s="2"/>
       <c r="AK131" s="2"/>
     </row>
-    <row r="132" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3833,7 +3979,7 @@
       <c r="AJ132" s="2"/>
       <c r="AK132" s="2"/>
     </row>
-    <row r="133" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3872,7 +4018,7 @@
       <c r="AJ133" s="2"/>
       <c r="AK133" s="2"/>
     </row>
-    <row r="134" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3911,7 +4057,7 @@
       <c r="AJ134" s="2"/>
       <c r="AK134" s="2"/>
     </row>
-    <row r="135" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3950,7 +4096,7 @@
       <c r="AJ135" s="2"/>
       <c r="AK135" s="2"/>
     </row>
-    <row r="136" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3989,7 +4135,7 @@
       <c r="AJ136" s="2"/>
       <c r="AK136" s="2"/>
     </row>
-    <row r="137" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -4028,7 +4174,7 @@
       <c r="AJ137" s="2"/>
       <c r="AK137" s="2"/>
     </row>
-    <row r="138" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -4067,7 +4213,7 @@
       <c r="AJ138" s="2"/>
       <c r="AK138" s="2"/>
     </row>
-    <row r="139" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -4106,7 +4252,7 @@
       <c r="AJ139" s="2"/>
       <c r="AK139" s="2"/>
     </row>
-    <row r="140" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -4145,7 +4291,7 @@
       <c r="AJ140" s="2"/>
       <c r="AK140" s="2"/>
     </row>
-    <row r="141" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -4184,7 +4330,7 @@
       <c r="AJ141" s="2"/>
       <c r="AK141" s="2"/>
     </row>
-    <row r="142" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -4223,7 +4369,7 @@
       <c r="AJ142" s="2"/>
       <c r="AK142" s="2"/>
     </row>
-    <row r="143" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -4262,7 +4408,7 @@
       <c r="AJ143" s="2"/>
       <c r="AK143" s="2"/>
     </row>
-    <row r="144" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -4301,7 +4447,7 @@
       <c r="AJ144" s="2"/>
       <c r="AK144" s="2"/>
     </row>
-    <row r="145" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -4348,15 +4494,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40">
@@ -4367,7 +4504,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100121BB807B7133F4E97909F1E9C01581D" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="61d18d9999cc13d434223f9e3875bfe4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40" xmlns:ns3="c3032618-4d7f-458c-877f-4482583a752b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a4acd2033efad1f0dccd4f0684ff0f6" ns2:_="" ns3:_="">
     <xsd:import namespace="fc6debfa-00d5-40a8-9b82-61b9f2aa7d40"/>
@@ -4568,15 +4705,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABBE2C1-0B0B-4891-85CC-3124E2C37EEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18CFC937-C7E0-4A5C-9F9E-E1CFACFBA053}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4593,7 +4731,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97D496CE-223B-4967-8C89-F3A8C84F0D3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4610,4 +4748,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABBE2C1-0B0B-4891-85CC-3124E2C37EEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>